<commit_message>
v1.1.0 - update to act-1.8.8-RC4; fix #2 This site cannot be reached after i hit the download button
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/com/pixolut/sonar/Report/report.xlsx
+++ b/src/main/resources/excel/com/pixolut/sonar/Report/report.xlsx
@@ -70,7 +70,7 @@
     <t xml:space="preserve">Severity</t>
   </si>
   <si>
-    <t xml:space="preserve">Component</t>
+    <t xml:space="preserve">Source</t>
   </si>
   <si>
     <t xml:space="preserve">Message</t>
@@ -82,7 +82,7 @@
     <t xml:space="preserve">${issue.severity}</t>
   </si>
   <si>
-    <t xml:space="preserve">${issue.component}</t>
+    <t xml:space="preserve">${issue.source}</t>
   </si>
   <si>
     <t xml:space="preserve">${issue.message}</t>
@@ -104,6 +104,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -126,6 +127,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -133,6 +135,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
@@ -302,19 +305,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D65536"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="87.5306122448979"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.0459183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.7959183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="58.3163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -337,7 +339,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>5</v>
       </c>
@@ -351,7 +353,6 @@
         <v>8</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.699305555555555" right="0.699305555555555" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -377,7 +378,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>